<commit_message>
Add a count in the "Action" column
If a SAN, then "Action" value will be "Add 1" or "Subtract" one.
If any other item, it will be "Add [total]", "Subtract [total]"
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -300,7 +300,7 @@
         </is>
       </c>
       <c r="B2" s="4" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>17</v>
@@ -373,8 +373,12 @@
           <t xml:space="preserve">Laptop Charger </t>
         </is>
       </c>
-      <c r="B8" s="4" t="n"/>
-      <c r="C8" s="4" t="n"/>
+      <c r="B8" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="3" t="inlineStr">
@@ -383,10 +387,10 @@
         </is>
       </c>
       <c r="B9" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
@@ -422,7 +426,7 @@
         </is>
       </c>
       <c r="B12" s="4" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>9</v>
@@ -509,7 +513,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A68" sqref="A68:XFD68"/>
@@ -1933,6 +1937,445 @@
       <c r="C67" t="inlineStr">
         <is>
           <t>add</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:18:00</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Laptop Charger </t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:18:10</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Laptop Charger </t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>add 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:18:26</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>SAN124323</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:18:30</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>SAN124354</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:18:38</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>USB DVD-RW Drive</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:18:48</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>USB DVD-RW Drive</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:22:16</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>SAN124354</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:22:43</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Laptop Charger </t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:28:21</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>add</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>SAN123456</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:28:27</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>subtract</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>SAN123456</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:47:39</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>SAN13579</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:47:48</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>SAN13578</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:47:55</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:48:02</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:58:04</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>SAN124578</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:58:20</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:58:48</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>SAN124589</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-01-14 14:59:05</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-01-14 15:06:14</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>SAN223344</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-01-14 15:06:19</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>SAN445566</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-01-14 15:06:40</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>SAN223344</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-01-14 15:06:50</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>SAN445566</t>
         </is>
       </c>
     </row>
@@ -2373,7 +2816,6 @@
           <t>add</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11" ht="12.75" customHeight="1"/>
     <row r="12" ht="12.75" customHeight="1"/>
@@ -2654,7 +3096,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="A2:C4"/>
@@ -3574,7 +4016,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>SAN106026</t>
+          <t>SAN106008</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -3584,48 +4026,48 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2024-01-10 16:52:08</t>
+          <t>2024-01-10 16:52:17</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>SAN106008</t>
+          <t>SAN111111</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Laptop x360 G8</t>
+          <t>Laptop 840 G10</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2024-01-10 16:52:17</t>
+          <t>2024-01-11 12:06:10</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>SAN111111</t>
+          <t>SAN120950</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>Laptop 840 G9</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2024-01-11 12:06:10</t>
+          <t>2024-01-12 10:54:13</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>SAN120950</t>
+          <t>SAN120864</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -3634,23 +4076,6 @@
         </is>
       </c>
       <c r="C58" t="inlineStr">
-        <is>
-          <t>2024-01-12 10:54:13</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>SAN120864</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Laptop 840 G9</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
         <is>
           <t>2024-01-12 10:54:20</t>
         </is>

</xml_diff>

<commit_message>
Revert v2.10, reject b2.11, add item column to timesheets sheets
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="All SANs" sheetId="1" state="visible" r:id="rId1"/>
@@ -1297,10 +1297,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1344,8 +1344,12 @@
           <t>Dock Thunderbolt Slim</t>
         </is>
       </c>
-      <c r="B3" s="9" t="n"/>
-      <c r="C3" s="9" t="n"/>
+      <c r="B3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="7">
       <c r="A4" s="11" t="inlineStr">
@@ -1402,126 +1406,139 @@
     <row r="8" ht="12.75" customHeight="1" s="7">
       <c r="A8" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Laptop Charger </t>
+          <t>Laptop Bag</t>
         </is>
       </c>
       <c r="B8" s="9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C8" s="9" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="7">
       <c r="A9" s="11" t="inlineStr">
         <is>
-          <t>Laptop x360 G8</t>
+          <t xml:space="preserve">Laptop Charger </t>
         </is>
       </c>
       <c r="B9" s="9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" s="9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="7">
       <c r="A10" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Monitor 24” </t>
+          <t>Laptop x360 G8</t>
         </is>
       </c>
       <c r="B10" s="9" t="n">
         <v>4</v>
       </c>
       <c r="C10" s="9" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="7">
       <c r="A11" s="11" t="inlineStr">
         <is>
-          <t>Monitor 34” Ultrawide</t>
+          <t xml:space="preserve">Monitor 24” </t>
         </is>
       </c>
       <c r="B11" s="9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" s="9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="7">
       <c r="A12" s="11" t="inlineStr">
         <is>
-          <t>USB DVD-RW Drive</t>
+          <t>Monitor 34” Ultrawide</t>
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C12" s="9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="7">
       <c r="A13" s="11" t="inlineStr">
         <is>
-          <t>Wired Headset Poly</t>
+          <t>USB DVD-RW Drive</t>
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C13" s="9" t="n">
-        <v>63</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="7">
       <c r="A14" s="11" t="inlineStr">
         <is>
-          <t>Wired Keyboard</t>
+          <t>Wired Headset Poly</t>
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C14" s="9" t="n">
-        <v>36</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="7">
       <c r="A15" s="11" t="inlineStr">
         <is>
-          <t>Wired Mouse</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="n"/>
-      <c r="C15" s="9" t="n"/>
+          <t>Wired Keyboard</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="7">
       <c r="A16" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wireless Headset Poly </t>
-        </is>
-      </c>
-      <c r="B16" s="9" t="n">
-        <v>14</v>
-      </c>
-      <c r="C16" s="9" t="n">
-        <v>13</v>
-      </c>
+          <t>Wired Mouse</t>
+        </is>
+      </c>
+      <c r="B16" s="9" t="n"/>
+      <c r="C16" s="9" t="n"/>
     </row>
     <row r="17" ht="12.75" customHeight="1" s="7">
       <c r="A17" s="11" t="inlineStr">
         <is>
+          <t xml:space="preserve">Wireless Headset Poly </t>
+        </is>
+      </c>
+      <c r="B17" s="9" t="n">
+        <v>13</v>
+      </c>
+      <c r="C17" s="9" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" ht="12.75" customHeight="1" s="7">
+      <c r="A18" s="11" t="inlineStr">
+        <is>
           <t>Wireless KB &amp; Mouse</t>
         </is>
       </c>
-      <c r="B17" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="C17" s="9" t="n">
+      <c r="B18" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1546,7 +1563,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
@@ -3874,7 +3891,7 @@
         </is>
       </c>
     </row>
-    <row r="113">
+    <row r="113" ht="12.75" customHeight="1" s="7">
       <c r="A113" s="10" t="inlineStr">
         <is>
           <t>2024-01-31 21:18:42</t>
@@ -3890,9 +3907,8 @@
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D113" s="10" t="inlineStr"/>
-    </row>
-    <row r="114">
+    </row>
+    <row r="114" ht="12.75" customHeight="1" s="7">
       <c r="A114" s="10" t="inlineStr">
         <is>
           <t>2024-01-31 21:20:15</t>
@@ -3908,9 +3924,8 @@
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D114" s="10" t="inlineStr"/>
-    </row>
-    <row r="115">
+    </row>
+    <row r="115" ht="12.75" customHeight="1" s="7">
       <c r="A115" s="10" t="inlineStr">
         <is>
           <t>2024-01-31 21:24:35</t>
@@ -3926,25 +3941,144 @@
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D115" s="10" t="inlineStr"/>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
+    </row>
+    <row r="116" ht="12.75" customHeight="1" s="7">
+      <c r="A116" s="10" t="inlineStr">
         <is>
           <t>2024-01-31 22:08:34</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
+      <c r="B116" s="10" t="inlineStr">
         <is>
           <t>Wired Headset Poly</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr">
+      <c r="C116" s="10" t="inlineStr">
         <is>
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D116" t="inlineStr"/>
+    </row>
+    <row r="117" ht="12.75" customHeight="1" s="7">
+      <c r="A117" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-01 22:38:08</t>
+        </is>
+      </c>
+      <c r="B117" s="10" t="inlineStr">
+        <is>
+          <t>Wired Headset Poly</t>
+        </is>
+      </c>
+      <c r="C117" s="10" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="118" ht="12.75" customHeight="1" s="7">
+      <c r="A118" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-01 22:38:23</t>
+        </is>
+      </c>
+      <c r="B118" s="10" t="inlineStr">
+        <is>
+          <t>Wireless KB &amp; Mouse</t>
+        </is>
+      </c>
+      <c r="C118" s="10" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="119" ht="12.75" customHeight="1" s="7">
+      <c r="A119" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-01 22:38:23</t>
+        </is>
+      </c>
+      <c r="B119" s="10" t="inlineStr">
+        <is>
+          <t>Wireless KB &amp; Mouse</t>
+        </is>
+      </c>
+      <c r="C119" s="10" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="120" ht="12.75" customHeight="1" s="7">
+      <c r="A120" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-01 22:38:27</t>
+        </is>
+      </c>
+      <c r="B120" s="10" t="inlineStr">
+        <is>
+          <t>Wireless KB &amp; Mouse</t>
+        </is>
+      </c>
+      <c r="C120" s="10" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="121" ht="12.75" customHeight="1" s="7">
+      <c r="A121" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-01 22:38:27</t>
+        </is>
+      </c>
+      <c r="B121" s="10" t="inlineStr">
+        <is>
+          <t>Wireless KB &amp; Mouse</t>
+        </is>
+      </c>
+      <c r="C121" s="10" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-02 00:48:37</t>
+        </is>
+      </c>
+      <c r="B122" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wireless Headset Poly </t>
+        </is>
+      </c>
+      <c r="C122" s="10" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D122" s="10" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2024-02-02 00:51:47</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt Slim</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr"/>
     </row>
     <row r="1048576" ht="12.75" customHeight="1" s="7"/>
   </sheetData>
@@ -4465,9 +4599,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4505,7 +4639,7 @@
           <t>TASK-44458543</t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr"/>
+      <c r="C2" s="10" t="n"/>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="7">
       <c r="A3" s="10" t="inlineStr">
@@ -4518,7 +4652,7 @@
           <t>TASK-485737</t>
         </is>
       </c>
-      <c r="C3" s="10" t="inlineStr"/>
+      <c r="C3" s="10" t="n"/>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="7">
       <c r="A4" s="10" t="inlineStr">
@@ -4531,27 +4665,98 @@
           <t>TASK-3434343</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr"/>
+      <c r="C4" s="10" t="n"/>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="7">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>33333</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>TASK33333</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-    </row>
-    <row r="6" ht="12.75" customHeight="1" s="7"/>
-    <row r="7" ht="12.75" customHeight="1" s="7"/>
-    <row r="8" ht="12.75" customHeight="1" s="7"/>
-    <row r="1048574" ht="12.8" customHeight="1" s="7"/>
-    <row r="1048575" ht="12.8" customHeight="1" s="7"/>
-    <row r="1048576" ht="12.8" customHeight="1" s="7"/>
+      <c r="C5" s="10" t="n"/>
+    </row>
+    <row r="6" ht="12.75" customHeight="1" s="7">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>cfc323</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>TASK4343434</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1" s="7">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>f35c5c</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="inlineStr">
+        <is>
+          <t>TASK554545454</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="7">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>2323</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>TASKr544vvvv</t>
+        </is>
+      </c>
+      <c r="C8" s="10" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>43545</t>
+        </is>
+      </c>
+      <c r="B9" s="10" t="inlineStr">
+        <is>
+          <t>TASKdfdf3</t>
+        </is>
+      </c>
+      <c r="C9" s="10" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>23232</t>
+        </is>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>TASKcvvcvcv</t>
+        </is>
+      </c>
+      <c r="C10" s="10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>434344</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>TASKbvbv45r</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+    </row>
+    <row r="1048576" ht="12.75" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Fix Serial # AlphaNumerical input, ServiceNow # Numerical Input
Clean up code
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="All SANs" sheetId="1" state="visible" r:id="rId1"/>
@@ -308,8 +308,8 @@
   </sheetPr>
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -335,14 +335,26 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1" s="7">
-      <c r="A2" s="9" t="n"/>
-      <c r="B2" s="9" t="n"/>
-      <c r="C2" s="9" t="n"/>
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>SAN125045</t>
+        </is>
+      </c>
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C2" s="9" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:29:34</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="7">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>SAN125045</t>
+          <t>SAN125047</t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
@@ -352,14 +364,14 @@
       </c>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:29:34</t>
+          <t>2024-01-10 16:29:47</t>
         </is>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="7">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>SAN125047</t>
+          <t>SAN125043</t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
@@ -369,14 +381,14 @@
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:29:47</t>
+          <t>2024-01-10 16:29:53</t>
         </is>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="7">
       <c r="A5" s="9" t="inlineStr">
         <is>
-          <t>SAN125043</t>
+          <t>SAN125067</t>
         </is>
       </c>
       <c r="B5" s="9" t="inlineStr">
@@ -386,14 +398,14 @@
       </c>
       <c r="C5" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:29:53</t>
+          <t>2024-01-10 16:29:56</t>
         </is>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="7">
       <c r="A6" s="9" t="inlineStr">
         <is>
-          <t>SAN125067</t>
+          <t>SAN125078</t>
         </is>
       </c>
       <c r="B6" s="9" t="inlineStr">
@@ -403,14 +415,14 @@
       </c>
       <c r="C6" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:29:56</t>
+          <t>2024-01-10 16:30:01</t>
         </is>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="7">
       <c r="A7" s="9" t="inlineStr">
         <is>
-          <t>SAN125078</t>
+          <t>SAN125060</t>
         </is>
       </c>
       <c r="B7" s="9" t="inlineStr">
@@ -420,14 +432,14 @@
       </c>
       <c r="C7" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:30:01</t>
+          <t>2024-01-10 16:30:05</t>
         </is>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="7">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t>SAN125060</t>
+          <t>SAN125059</t>
         </is>
       </c>
       <c r="B8" s="9" t="inlineStr">
@@ -437,14 +449,14 @@
       </c>
       <c r="C8" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:30:05</t>
+          <t>2024-01-10 16:30:11</t>
         </is>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="7">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>SAN125059</t>
+          <t>SAN125065</t>
         </is>
       </c>
       <c r="B9" s="9" t="inlineStr">
@@ -454,14 +466,14 @@
       </c>
       <c r="C9" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:30:11</t>
+          <t>2024-01-10 16:30:17</t>
         </is>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="7">
       <c r="A10" s="9" t="inlineStr">
         <is>
-          <t>SAN125065</t>
+          <t>SAN125063</t>
         </is>
       </c>
       <c r="B10" s="9" t="inlineStr">
@@ -471,14 +483,14 @@
       </c>
       <c r="C10" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:30:17</t>
+          <t>2024-01-10 16:30:23</t>
         </is>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="7">
       <c r="A11" s="9" t="inlineStr">
         <is>
-          <t>SAN125063</t>
+          <t>SAN125064</t>
         </is>
       </c>
       <c r="B11" s="9" t="inlineStr">
@@ -488,14 +500,14 @@
       </c>
       <c r="C11" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:30:23</t>
+          <t>2024-01-10 16:30:29</t>
         </is>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="7">
       <c r="A12" s="9" t="inlineStr">
         <is>
-          <t>SAN125064</t>
+          <t>SAN125054</t>
         </is>
       </c>
       <c r="B12" s="9" t="inlineStr">
@@ -505,14 +517,14 @@
       </c>
       <c r="C12" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:30:29</t>
+          <t>2024-01-10 16:30:34</t>
         </is>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="7">
       <c r="A13" s="9" t="inlineStr">
         <is>
-          <t>SAN125054</t>
+          <t>SAN125061</t>
         </is>
       </c>
       <c r="B13" s="9" t="inlineStr">
@@ -522,14 +534,14 @@
       </c>
       <c r="C13" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:30:34</t>
+          <t>2024-01-10 16:30:45</t>
         </is>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="7">
       <c r="A14" s="9" t="inlineStr">
         <is>
-          <t>SAN125061</t>
+          <t>SAN125071</t>
         </is>
       </c>
       <c r="B14" s="9" t="inlineStr">
@@ -539,14 +551,14 @@
       </c>
       <c r="C14" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:30:45</t>
+          <t>2024-01-10 16:30:59</t>
         </is>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="7">
       <c r="A15" s="9" t="inlineStr">
         <is>
-          <t>SAN125071</t>
+          <t>SAN125072</t>
         </is>
       </c>
       <c r="B15" s="9" t="inlineStr">
@@ -556,14 +568,14 @@
       </c>
       <c r="C15" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:30:59</t>
+          <t>2024-01-10 16:31:09</t>
         </is>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="7">
       <c r="A16" s="9" t="inlineStr">
         <is>
-          <t>SAN125072</t>
+          <t>SAN125053</t>
         </is>
       </c>
       <c r="B16" s="9" t="inlineStr">
@@ -573,14 +585,14 @@
       </c>
       <c r="C16" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:31:09</t>
+          <t>2024-01-10 16:31:14</t>
         </is>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" s="7">
       <c r="A17" s="9" t="inlineStr">
         <is>
-          <t>SAN125053</t>
+          <t>SAN125077</t>
         </is>
       </c>
       <c r="B17" s="9" t="inlineStr">
@@ -590,14 +602,14 @@
       </c>
       <c r="C17" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:31:14</t>
+          <t>2024-01-10 16:31:23</t>
         </is>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1" s="7">
       <c r="A18" s="9" t="inlineStr">
         <is>
-          <t>SAN125077</t>
+          <t>SAN125076</t>
         </is>
       </c>
       <c r="B18" s="9" t="inlineStr">
@@ -607,31 +619,31 @@
       </c>
       <c r="C18" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:31:23</t>
+          <t>2024-01-10 16:31:28</t>
         </is>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1" s="7">
       <c r="A19" s="9" t="inlineStr">
         <is>
-          <t>SAN125076</t>
+          <t>SAN122589</t>
         </is>
       </c>
       <c r="B19" s="9" t="inlineStr">
         <is>
-          <t>Desktop Mini G9</t>
+          <t>Laptop 840 G10</t>
         </is>
       </c>
       <c r="C19" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:31:28</t>
+          <t>2024-01-10 16:39:28</t>
         </is>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1" s="7">
       <c r="A20" s="9" t="inlineStr">
         <is>
-          <t>SAN122589</t>
+          <t>SAN122596</t>
         </is>
       </c>
       <c r="B20" s="9" t="inlineStr">
@@ -641,14 +653,14 @@
       </c>
       <c r="C20" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:39:28</t>
+          <t>2024-01-10 16:39:32</t>
         </is>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1" s="7">
       <c r="A21" s="9" t="inlineStr">
         <is>
-          <t>SAN122596</t>
+          <t>SAN122603</t>
         </is>
       </c>
       <c r="B21" s="9" t="inlineStr">
@@ -658,14 +670,14 @@
       </c>
       <c r="C21" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:39:32</t>
+          <t>2024-01-10 16:39:40</t>
         </is>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1" s="7">
       <c r="A22" s="9" t="inlineStr">
         <is>
-          <t>SAN122603</t>
+          <t>SAN122611</t>
         </is>
       </c>
       <c r="B22" s="9" t="inlineStr">
@@ -675,14 +687,14 @@
       </c>
       <c r="C22" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:39:40</t>
+          <t>2024-01-10 16:39:47</t>
         </is>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1" s="7">
       <c r="A23" s="9" t="inlineStr">
         <is>
-          <t>SAN122611</t>
+          <t>SAN122590</t>
         </is>
       </c>
       <c r="B23" s="9" t="inlineStr">
@@ -692,14 +704,14 @@
       </c>
       <c r="C23" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:39:47</t>
+          <t>2024-01-10 16:39:53</t>
         </is>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1" s="7">
       <c r="A24" s="9" t="inlineStr">
         <is>
-          <t>SAN122590</t>
+          <t>SAN122593</t>
         </is>
       </c>
       <c r="B24" s="9" t="inlineStr">
@@ -709,14 +721,14 @@
       </c>
       <c r="C24" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:39:53</t>
+          <t>2024-01-10 16:40:16</t>
         </is>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1" s="7">
       <c r="A25" s="9" t="inlineStr">
         <is>
-          <t>SAN122593</t>
+          <t>SAN122597</t>
         </is>
       </c>
       <c r="B25" s="9" t="inlineStr">
@@ -726,14 +738,14 @@
       </c>
       <c r="C25" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:40:16</t>
+          <t>2024-01-10 16:40:40</t>
         </is>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1" s="7">
       <c r="A26" s="9" t="inlineStr">
         <is>
-          <t>SAN122597</t>
+          <t>SAN122602</t>
         </is>
       </c>
       <c r="B26" s="9" t="inlineStr">
@@ -743,14 +755,14 @@
       </c>
       <c r="C26" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:40:40</t>
+          <t>2024-01-10 16:40:49</t>
         </is>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1" s="7">
       <c r="A27" s="9" t="inlineStr">
         <is>
-          <t>SAN122602</t>
+          <t>SAN122610</t>
         </is>
       </c>
       <c r="B27" s="9" t="inlineStr">
@@ -760,14 +772,14 @@
       </c>
       <c r="C27" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:40:49</t>
+          <t>2024-01-10 16:40:53</t>
         </is>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1" s="7">
       <c r="A28" s="9" t="inlineStr">
         <is>
-          <t>SAN122610</t>
+          <t>SAN122599</t>
         </is>
       </c>
       <c r="B28" s="9" t="inlineStr">
@@ -777,14 +789,14 @@
       </c>
       <c r="C28" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:40:53</t>
+          <t>2024-01-10 16:40:58</t>
         </is>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1" s="7">
       <c r="A29" s="9" t="inlineStr">
         <is>
-          <t>SAN122599</t>
+          <t>SAN122592</t>
         </is>
       </c>
       <c r="B29" s="9" t="inlineStr">
@@ -794,14 +806,14 @@
       </c>
       <c r="C29" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:40:58</t>
+          <t>2024-01-10 16:41:03</t>
         </is>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1" s="7">
       <c r="A30" s="9" t="inlineStr">
         <is>
-          <t>SAN122592</t>
+          <t>SAN122607</t>
         </is>
       </c>
       <c r="B30" s="9" t="inlineStr">
@@ -811,14 +823,14 @@
       </c>
       <c r="C30" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:41:03</t>
+          <t>2024-01-10 16:41:08</t>
         </is>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1" s="7">
       <c r="A31" s="9" t="inlineStr">
         <is>
-          <t>SAN122607</t>
+          <t>SAN122608</t>
         </is>
       </c>
       <c r="B31" s="9" t="inlineStr">
@@ -828,14 +840,14 @@
       </c>
       <c r="C31" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:41:08</t>
+          <t>2024-01-10 16:41:15</t>
         </is>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1" s="7">
       <c r="A32" s="9" t="inlineStr">
         <is>
-          <t>SAN122608</t>
+          <t>SAN122598</t>
         </is>
       </c>
       <c r="B32" s="9" t="inlineStr">
@@ -845,14 +857,14 @@
       </c>
       <c r="C32" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:41:15</t>
+          <t>2024-01-10 16:41:20</t>
         </is>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1" s="7">
       <c r="A33" s="9" t="inlineStr">
         <is>
-          <t>SAN122598</t>
+          <t>SAN122591</t>
         </is>
       </c>
       <c r="B33" s="9" t="inlineStr">
@@ -862,14 +874,14 @@
       </c>
       <c r="C33" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:41:20</t>
+          <t>2024-01-10 16:41:26</t>
         </is>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1" s="7">
       <c r="A34" s="9" t="inlineStr">
         <is>
-          <t>SAN122591</t>
+          <t>SAN122613</t>
         </is>
       </c>
       <c r="B34" s="9" t="inlineStr">
@@ -879,14 +891,14 @@
       </c>
       <c r="C34" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:41:26</t>
+          <t>2024-01-10 16:41:42</t>
         </is>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1" s="7">
       <c r="A35" s="9" t="inlineStr">
         <is>
-          <t>SAN122613</t>
+          <t>SAN122604</t>
         </is>
       </c>
       <c r="B35" s="9" t="inlineStr">
@@ -896,14 +908,14 @@
       </c>
       <c r="C35" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:41:42</t>
+          <t>2024-01-10 16:41:50</t>
         </is>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1" s="7">
       <c r="A36" s="9" t="inlineStr">
         <is>
-          <t>SAN122604</t>
+          <t>SAN122605</t>
         </is>
       </c>
       <c r="B36" s="9" t="inlineStr">
@@ -913,14 +925,14 @@
       </c>
       <c r="C36" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:41:50</t>
+          <t>2024-01-10 16:42:01</t>
         </is>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1" s="7">
       <c r="A37" s="9" t="inlineStr">
         <is>
-          <t>SAN122605</t>
+          <t>SAN122606</t>
         </is>
       </c>
       <c r="B37" s="9" t="inlineStr">
@@ -930,14 +942,14 @@
       </c>
       <c r="C37" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:42:01</t>
+          <t>2024-01-10 16:42:07</t>
         </is>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1" s="7">
       <c r="A38" s="9" t="inlineStr">
         <is>
-          <t>SAN122606</t>
+          <t>SAN122601</t>
         </is>
       </c>
       <c r="B38" s="9" t="inlineStr">
@@ -947,14 +959,14 @@
       </c>
       <c r="C38" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:42:07</t>
+          <t>2024-01-10 16:42:13</t>
         </is>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1" s="7">
       <c r="A39" s="9" t="inlineStr">
         <is>
-          <t>SAN122601</t>
+          <t>SAN122595</t>
         </is>
       </c>
       <c r="B39" s="9" t="inlineStr">
@@ -964,14 +976,14 @@
       </c>
       <c r="C39" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:42:13</t>
+          <t>2024-01-10 16:42:19</t>
         </is>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1" s="7">
       <c r="A40" s="9" t="inlineStr">
         <is>
-          <t>SAN122595</t>
+          <t>SAN122609</t>
         </is>
       </c>
       <c r="B40" s="9" t="inlineStr">
@@ -981,14 +993,14 @@
       </c>
       <c r="C40" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:42:19</t>
+          <t>2024-01-10 16:43:15</t>
         </is>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1" s="7">
       <c r="A41" s="9" t="inlineStr">
         <is>
-          <t>SAN122609</t>
+          <t>SAN122594</t>
         </is>
       </c>
       <c r="B41" s="9" t="inlineStr">
@@ -998,14 +1010,14 @@
       </c>
       <c r="C41" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:43:15</t>
+          <t>2024-01-10 16:43:21</t>
         </is>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1" s="7">
       <c r="A42" s="9" t="inlineStr">
         <is>
-          <t>SAN122594</t>
+          <t>SAN122612</t>
         </is>
       </c>
       <c r="B42" s="9" t="inlineStr">
@@ -1015,14 +1027,14 @@
       </c>
       <c r="C42" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:43:21</t>
+          <t>2024-01-10 16:43:39</t>
         </is>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1" s="7">
       <c r="A43" s="9" t="inlineStr">
         <is>
-          <t>SAN122612</t>
+          <t>SAN122304</t>
         </is>
       </c>
       <c r="B43" s="9" t="inlineStr">
@@ -1032,14 +1044,14 @@
       </c>
       <c r="C43" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:43:39</t>
+          <t>2024-01-10 16:43:46</t>
         </is>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1" s="7">
       <c r="A44" s="9" t="inlineStr">
         <is>
-          <t>SAN122304</t>
+          <t>SAN122305</t>
         </is>
       </c>
       <c r="B44" s="9" t="inlineStr">
@@ -1049,14 +1061,14 @@
       </c>
       <c r="C44" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:43:46</t>
+          <t>2024-01-10 16:43:53</t>
         </is>
       </c>
     </row>
     <row r="45" ht="12.75" customHeight="1" s="7">
       <c r="A45" s="9" t="inlineStr">
         <is>
-          <t>SAN122305</t>
+          <t>SAN122600</t>
         </is>
       </c>
       <c r="B45" s="9" t="inlineStr">
@@ -1066,31 +1078,31 @@
       </c>
       <c r="C45" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:43:53</t>
+          <t>2024-01-10 16:44:23</t>
         </is>
       </c>
     </row>
     <row r="46" ht="12.75" customHeight="1" s="7">
       <c r="A46" s="9" t="inlineStr">
         <is>
-          <t>SAN122600</t>
+          <t>SAN121911</t>
         </is>
       </c>
       <c r="B46" s="9" t="inlineStr">
         <is>
-          <t>Laptop 840 G10</t>
+          <t>Laptop 840 G9</t>
         </is>
       </c>
       <c r="C46" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:44:23</t>
+          <t>2024-01-10 16:50:07</t>
         </is>
       </c>
     </row>
     <row r="47" ht="12.75" customHeight="1" s="7">
       <c r="A47" s="9" t="inlineStr">
         <is>
-          <t>SAN121911</t>
+          <t>SAN121929</t>
         </is>
       </c>
       <c r="B47" s="9" t="inlineStr">
@@ -1100,14 +1112,14 @@
       </c>
       <c r="C47" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:50:07</t>
+          <t>2024-01-10 16:50:29</t>
         </is>
       </c>
     </row>
     <row r="48" ht="12.75" customHeight="1" s="7">
       <c r="A48" s="9" t="inlineStr">
         <is>
-          <t>SAN121929</t>
+          <t>SAN120286</t>
         </is>
       </c>
       <c r="B48" s="9" t="inlineStr">
@@ -1117,14 +1129,14 @@
       </c>
       <c r="C48" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:50:29</t>
+          <t>2024-01-10 16:50:46</t>
         </is>
       </c>
     </row>
     <row r="49" ht="12.75" customHeight="1" s="7">
       <c r="A49" s="9" t="inlineStr">
         <is>
-          <t>SAN120286</t>
+          <t>SAN120342</t>
         </is>
       </c>
       <c r="B49" s="9" t="inlineStr">
@@ -1134,148 +1146,148 @@
       </c>
       <c r="C49" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:50:46</t>
+          <t>2024-01-10 16:50:57</t>
         </is>
       </c>
     </row>
     <row r="50" ht="12.75" customHeight="1" s="7">
       <c r="A50" s="9" t="inlineStr">
         <is>
-          <t>SAN120342</t>
+          <t>SAN106014</t>
         </is>
       </c>
       <c r="B50" s="9" t="inlineStr">
         <is>
-          <t>Laptop 840 G9</t>
+          <t>Laptop x360 G8</t>
         </is>
       </c>
       <c r="C50" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:50:57</t>
+          <t>2024-01-10 16:52:00</t>
         </is>
       </c>
     </row>
     <row r="51" ht="12.75" customHeight="1" s="7">
       <c r="A51" s="9" t="inlineStr">
         <is>
-          <t>SAN106013</t>
+          <t>SAN111111</t>
         </is>
       </c>
       <c r="B51" s="9" t="inlineStr">
         <is>
-          <t>Laptop x360 G8</t>
+          <t>Laptop 840 G10</t>
         </is>
       </c>
       <c r="C51" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:51:46</t>
+          <t>2024-01-11 12:06:10</t>
         </is>
       </c>
     </row>
     <row r="52" ht="12.75" customHeight="1" s="7">
       <c r="A52" s="9" t="inlineStr">
         <is>
-          <t>SAN106014</t>
+          <t>SAN120950</t>
         </is>
       </c>
       <c r="B52" s="9" t="inlineStr">
         <is>
-          <t>Laptop x360 G8</t>
+          <t>Laptop 840 G9</t>
         </is>
       </c>
       <c r="C52" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:52:00</t>
+          <t>2024-01-12 10:54:13</t>
         </is>
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1" s="7">
       <c r="A53" s="9" t="inlineStr">
         <is>
-          <t>SAN106008</t>
+          <t>SAN120864</t>
         </is>
       </c>
       <c r="B53" s="9" t="inlineStr">
         <is>
-          <t>Laptop x360 G8</t>
+          <t>Laptop 840 G9</t>
         </is>
       </c>
       <c r="C53" s="9" t="inlineStr">
         <is>
-          <t>2024-01-10 16:52:17</t>
+          <t>2024-01-12 10:54:20</t>
         </is>
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1" s="7">
-      <c r="A54" s="9" t="inlineStr">
-        <is>
-          <t>SAN111111</t>
-        </is>
-      </c>
-      <c r="B54" s="9" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C54" s="9" t="inlineStr">
-        <is>
-          <t>2024-01-11 12:06:10</t>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>SAN3333333</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:48:24</t>
         </is>
       </c>
     </row>
     <row r="55" ht="12.75" customHeight="1" s="7">
-      <c r="A55" s="9" t="inlineStr">
-        <is>
-          <t>SAN120950</t>
-        </is>
-      </c>
-      <c r="B55" s="9" t="inlineStr">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>SAN456123</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C55" s="9" t="inlineStr">
-        <is>
-          <t>2024-01-12 10:54:13</t>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:49:57</t>
         </is>
       </c>
     </row>
     <row r="56" ht="12.75" customHeight="1" s="7">
-      <c r="A56" s="9" t="inlineStr">
-        <is>
-          <t>SAN120864</t>
-        </is>
-      </c>
-      <c r="B56" s="9" t="inlineStr">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>SAN152646</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C56" s="9" t="inlineStr">
-        <is>
-          <t>2024-01-12 10:54:20</t>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:50:05</t>
         </is>
       </c>
     </row>
     <row r="57" ht="12.75" customHeight="1" s="7">
-      <c r="A57" s="9" t="inlineStr">
-        <is>
-          <t>SAN343434</t>
-        </is>
-      </c>
-      <c r="B57" s="9" t="inlineStr">
-        <is>
-          <t>Laptop 840 G9</t>
-        </is>
-      </c>
-      <c r="C57" s="9" t="inlineStr">
-        <is>
-          <t>2024-01-29 23:52:55</t>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>SAN44444444</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:50:17</t>
         </is>
       </c>
     </row>
     <row r="58" ht="12.75" customHeight="1" s="7"/>
-    <row r="59" ht="12.75" customHeight="1" s="7"/>
+    <row r="1048576" ht="12.8" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1299,7 +1311,7 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1345,10 +1357,10 @@
         </is>
       </c>
       <c r="B3" s="9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="7">
@@ -1358,10 +1370,10 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C4" s="9" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="7">
@@ -1371,10 +1383,10 @@
         </is>
       </c>
       <c r="B5" s="9" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C5" s="9" t="n">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="7">
@@ -1501,10 +1513,10 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C15" s="9" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="7">
@@ -1536,10 +1548,10 @@
         </is>
       </c>
       <c r="B18" s="9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" s="9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1563,7 +1575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
@@ -4044,7 +4056,7 @@
         </is>
       </c>
     </row>
-    <row r="122">
+    <row r="122" ht="12.75" customHeight="1" s="7">
       <c r="A122" s="10" t="inlineStr">
         <is>
           <t>2024-02-02 00:48:37</t>
@@ -4060,25 +4072,551 @@
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D122" s="10" t="inlineStr"/>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
+    </row>
+    <row r="123" ht="12.75" customHeight="1" s="7">
+      <c r="A123" s="10" t="inlineStr">
         <is>
           <t>2024-02-02 00:51:47</t>
         </is>
       </c>
-      <c r="B123" t="inlineStr">
+      <c r="B123" s="10" t="inlineStr">
         <is>
           <t>Dock Thunderbolt Slim</t>
         </is>
       </c>
-      <c r="C123" t="inlineStr">
+      <c r="C123" s="10" t="inlineStr">
         <is>
           <t>add 2</t>
         </is>
       </c>
-      <c r="D123" t="inlineStr"/>
+    </row>
+    <row r="124" ht="12.75" customHeight="1" s="7">
+      <c r="A124" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-02 19:08:36</t>
+        </is>
+      </c>
+      <c r="B124" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wireless Headset Poly </t>
+        </is>
+      </c>
+      <c r="C124" s="10" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="125" ht="12.75" customHeight="1" s="7">
+      <c r="A125" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-02 23:51:57</t>
+        </is>
+      </c>
+      <c r="B125" s="10" t="inlineStr">
+        <is>
+          <t>Wired Headset Poly</t>
+        </is>
+      </c>
+      <c r="C125" s="10" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:04:46</t>
+        </is>
+      </c>
+      <c r="B126" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wireless Headset Poly </t>
+        </is>
+      </c>
+      <c r="C126" s="10" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+      <c r="D126" s="10" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:42:30</t>
+        </is>
+      </c>
+      <c r="B127" s="10" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C127" s="10" t="inlineStr">
+        <is>
+          <t>add 5</t>
+        </is>
+      </c>
+      <c r="D127" s="10" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:42:30</t>
+        </is>
+      </c>
+      <c r="B128" s="10" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C128" s="10" t="inlineStr">
+        <is>
+          <t>add 5</t>
+        </is>
+      </c>
+      <c r="D128" s="10" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:42:35</t>
+        </is>
+      </c>
+      <c r="B129" s="10" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G2</t>
+        </is>
+      </c>
+      <c r="C129" s="10" t="inlineStr">
+        <is>
+          <t>add 5</t>
+        </is>
+      </c>
+      <c r="D129" s="10" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:42:35</t>
+        </is>
+      </c>
+      <c r="B130" s="10" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G2</t>
+        </is>
+      </c>
+      <c r="C130" s="10" t="inlineStr">
+        <is>
+          <t>add 5</t>
+        </is>
+      </c>
+      <c r="D130" s="10" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:48:19</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G2</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:48:19</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G2</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:48:24</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>SAN3333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:48:49</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>SAN343434</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:49:19</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>SAN106008</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:49:37</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>SAN106013</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:49:57</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>SAN456123</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:50:05</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>SAN152646</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:50:17</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>SAN44444444</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:54:22</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Wired Headset Poly</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:58:11</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt Slim</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:58:11</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt Slim</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:58:14</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Wired Keyboard</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:58:14</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Wired Keyboard</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:58:17</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Wireless KB &amp; Mouse</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:58:17</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Wireless KB &amp; Mouse</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>add 2</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2024-02-03 00:59:50</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>SAN123456</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2024-02-03 01:00:02</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>SAN123455</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2024-02-03 01:00:32</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>SAN123455</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2024-02-03 01:00:53</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>SAN123456</t>
+        </is>
+      </c>
     </row>
     <row r="1048576" ht="12.75" customHeight="1" s="7"/>
   </sheetData>
@@ -4323,7 +4861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
@@ -4563,7 +5101,23 @@
       </c>
       <c r="D12" s="9" t="n"/>
     </row>
-    <row r="13" ht="12.75" customHeight="1" s="7"/>
+    <row r="13" ht="12.75" customHeight="1" s="7">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-02 23:52:23</t>
+        </is>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wireless Headset Poly </t>
+        </is>
+      </c>
+      <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+    </row>
     <row r="14" ht="12.75" customHeight="1" s="7"/>
     <row r="15" ht="12.75" customHeight="1" s="7"/>
     <row r="16" ht="12.75" customHeight="1" s="7"/>
@@ -4599,10 +5153,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4715,9 +5269,9 @@
           <t>TASKr544vvvv</t>
         </is>
       </c>
-      <c r="C8" s="10" t="inlineStr"/>
-    </row>
-    <row r="9">
+      <c r="C8" s="10" t="n"/>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" s="7">
       <c r="A9" s="10" t="inlineStr">
         <is>
           <t>43545</t>
@@ -4728,9 +5282,9 @@
           <t>TASKdfdf3</t>
         </is>
       </c>
-      <c r="C9" s="10" t="inlineStr"/>
-    </row>
-    <row r="10">
+      <c r="C9" s="10" t="n"/>
+    </row>
+    <row r="10" ht="12.75" customHeight="1" s="7">
       <c r="A10" s="10" t="inlineStr">
         <is>
           <t>23232</t>
@@ -4741,20 +5295,108 @@
           <t>TASKcvvcvcv</t>
         </is>
       </c>
-      <c r="C10" s="10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="C10" s="10" t="n"/>
+    </row>
+    <row r="11" ht="12.75" customHeight="1" s="7">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>434344</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="10" t="inlineStr">
         <is>
           <t>TASKbvbv45r</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" s="10" t="n"/>
+    </row>
+    <row r="12" ht="12.75" customHeight="1" s="7">
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <t>ddd333</t>
+        </is>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>TASK334343</t>
+        </is>
+      </c>
+      <c r="C12" s="10" t="n"/>
+    </row>
+    <row r="13" ht="12.75" customHeight="1" s="7">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>ccc333</t>
+        </is>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>TASK1234567</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="12.75" customHeight="1" s="7">
+      <c r="A14" s="10" t="inlineStr">
+        <is>
+          <t>d4v4v4</t>
+        </is>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>TASKvvv444</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="inlineStr">
+        <is>
+          <t>vv49fj5</t>
+        </is>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>RITM2345678</t>
+        </is>
+      </c>
+      <c r="C15" s="10" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>g67ui8</t>
+        </is>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>TASK8885544</t>
+        </is>
+      </c>
+      <c r="C16" s="10" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>g55f5g</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>INC4545454</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>445vv4</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>dfdffdfffd</t>
+        </is>
+      </c>
     </row>
     <row r="1048576" ht="12.75" customHeight="1" s="7"/>
   </sheetData>

</xml_diff>

<commit_message>
Enforce 6-digit limit on SAN Input function
Currently no min/max character limit
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -306,7 +306,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1219,74 +1219,124 @@
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1" s="7">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="10" t="inlineStr">
         <is>
           <t>SAN3333333</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
+      <c r="B54" s="10" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C54" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:48:24</t>
         </is>
       </c>
     </row>
     <row r="55" ht="12.75" customHeight="1" s="7">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="10" t="inlineStr">
         <is>
           <t>SAN456123</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" s="10" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C55" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:49:57</t>
         </is>
       </c>
     </row>
     <row r="56" ht="12.75" customHeight="1" s="7">
-      <c r="A56" t="inlineStr">
+      <c r="A56" s="10" t="inlineStr">
         <is>
           <t>SAN152646</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B56" s="10" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C56" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:50:05</t>
         </is>
       </c>
     </row>
     <row r="57" ht="12.75" customHeight="1" s="7">
-      <c r="A57" t="inlineStr">
+      <c r="A57" s="10" t="inlineStr">
         <is>
           <t>SAN44444444</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
+      <c r="B57" s="10" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C57" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:50:17</t>
         </is>
       </c>
     </row>
-    <row r="58" ht="12.75" customHeight="1" s="7"/>
+    <row r="58" ht="12.75" customHeight="1" s="7">
+      <c r="A58" s="10" t="inlineStr">
+        <is>
+          <t>SAN44</t>
+        </is>
+      </c>
+      <c r="B58" s="10" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C58" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-03 21:12:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="10" t="inlineStr">
+        <is>
+          <t>SAN09090909</t>
+        </is>
+      </c>
+      <c r="B59" s="10" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C59" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-03 21:13:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>SAN222444</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:15:52</t>
+        </is>
+      </c>
+    </row>
     <row r="1048576" ht="12.8" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -1370,10 +1420,10 @@
         </is>
       </c>
       <c r="B4" s="9" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="9" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="7">
@@ -1513,10 +1563,10 @@
         </is>
       </c>
       <c r="B15" s="9" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="9" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="7">
@@ -1525,8 +1575,12 @@
           <t>Wired Mouse</t>
         </is>
       </c>
-      <c r="B16" s="9" t="n"/>
-      <c r="C16" s="9" t="n"/>
+      <c r="B16" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" s="7">
       <c r="A17" s="11" t="inlineStr">
@@ -1575,7 +1629,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D164"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
@@ -4215,408 +4269,688 @@
       <c r="D130" s="10" t="inlineStr"/>
     </row>
     <row r="131">
-      <c r="A131" t="inlineStr">
+      <c r="A131" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:48:19</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
+      <c r="B131" s="10" t="inlineStr">
         <is>
           <t>Dock Thunderbolt G2</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
+      <c r="C131" s="10" t="inlineStr">
         <is>
           <t>add 1</t>
         </is>
       </c>
-      <c r="D131" t="inlineStr"/>
+      <c r="D131" s="10" t="inlineStr"/>
     </row>
     <row r="132">
-      <c r="A132" t="inlineStr">
+      <c r="A132" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:48:19</t>
         </is>
       </c>
-      <c r="B132" t="inlineStr">
+      <c r="B132" s="10" t="inlineStr">
         <is>
           <t>Dock Thunderbolt G2</t>
         </is>
       </c>
-      <c r="C132" t="inlineStr">
+      <c r="C132" s="10" t="inlineStr">
         <is>
           <t>add 1</t>
         </is>
       </c>
-      <c r="D132" t="inlineStr"/>
+      <c r="D132" s="10" t="inlineStr"/>
     </row>
     <row r="133">
-      <c r="A133" t="inlineStr">
+      <c r="A133" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:48:24</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
+      <c r="B133" s="10" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C133" s="10" t="inlineStr">
         <is>
           <t>add 1</t>
         </is>
       </c>
-      <c r="D133" t="inlineStr">
+      <c r="D133" s="10" t="inlineStr">
         <is>
           <t>SAN3333333</t>
         </is>
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="inlineStr">
+      <c r="A134" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:48:49</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr">
+      <c r="B134" s="10" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C134" t="inlineStr">
+      <c r="C134" s="10" t="inlineStr">
         <is>
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D134" t="inlineStr">
+      <c r="D134" s="10" t="inlineStr">
         <is>
           <t>SAN343434</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
+      <c r="A135" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:49:19</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr">
+      <c r="B135" s="10" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C135" t="inlineStr">
+      <c r="C135" s="10" t="inlineStr">
         <is>
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D135" t="inlineStr">
+      <c r="D135" s="10" t="inlineStr">
         <is>
           <t>SAN106008</t>
         </is>
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="inlineStr">
+      <c r="A136" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:49:37</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr">
+      <c r="B136" s="10" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C136" t="inlineStr">
+      <c r="C136" s="10" t="inlineStr">
         <is>
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D136" t="inlineStr">
+      <c r="D136" s="10" t="inlineStr">
         <is>
           <t>SAN106013</t>
         </is>
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="inlineStr">
+      <c r="A137" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:49:57</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr">
+      <c r="B137" s="10" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C137" t="inlineStr">
+      <c r="C137" s="10" t="inlineStr">
         <is>
           <t>add 1</t>
         </is>
       </c>
-      <c r="D137" t="inlineStr">
+      <c r="D137" s="10" t="inlineStr">
         <is>
           <t>SAN456123</t>
         </is>
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr">
+      <c r="A138" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:50:05</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
+      <c r="B138" s="10" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C138" t="inlineStr">
+      <c r="C138" s="10" t="inlineStr">
         <is>
           <t>add 1</t>
         </is>
       </c>
-      <c r="D138" t="inlineStr">
+      <c r="D138" s="10" t="inlineStr">
         <is>
           <t>SAN152646</t>
         </is>
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr">
+      <c r="A139" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:50:17</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
+      <c r="B139" s="10" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C139" s="10" t="inlineStr">
         <is>
           <t>add 1</t>
         </is>
       </c>
-      <c r="D139" t="inlineStr">
+      <c r="D139" s="10" t="inlineStr">
         <is>
           <t>SAN44444444</t>
         </is>
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
+      <c r="A140" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:54:22</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
+      <c r="B140" s="10" t="inlineStr">
         <is>
           <t>Wired Headset Poly</t>
         </is>
       </c>
-      <c r="C140" t="inlineStr">
+      <c r="C140" s="10" t="inlineStr">
         <is>
           <t>subtract 2</t>
         </is>
       </c>
-      <c r="D140" t="inlineStr"/>
+      <c r="D140" s="10" t="inlineStr"/>
     </row>
     <row r="141">
-      <c r="A141" t="inlineStr">
+      <c r="A141" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:58:11</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
+      <c r="B141" s="10" t="inlineStr">
         <is>
           <t>Dock Thunderbolt Slim</t>
         </is>
       </c>
-      <c r="C141" t="inlineStr">
+      <c r="C141" s="10" t="inlineStr">
         <is>
           <t>add 2</t>
         </is>
       </c>
-      <c r="D141" t="inlineStr"/>
+      <c r="D141" s="10" t="inlineStr"/>
     </row>
     <row r="142">
-      <c r="A142" t="inlineStr">
+      <c r="A142" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:58:11</t>
         </is>
       </c>
-      <c r="B142" t="inlineStr">
+      <c r="B142" s="10" t="inlineStr">
         <is>
           <t>Dock Thunderbolt Slim</t>
         </is>
       </c>
-      <c r="C142" t="inlineStr">
+      <c r="C142" s="10" t="inlineStr">
         <is>
           <t>add 2</t>
         </is>
       </c>
-      <c r="D142" t="inlineStr"/>
+      <c r="D142" s="10" t="inlineStr"/>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr">
+      <c r="A143" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:58:14</t>
         </is>
       </c>
-      <c r="B143" t="inlineStr">
+      <c r="B143" s="10" t="inlineStr">
         <is>
           <t>Wired Keyboard</t>
         </is>
       </c>
-      <c r="C143" t="inlineStr">
+      <c r="C143" s="10" t="inlineStr">
         <is>
           <t>add 2</t>
         </is>
       </c>
-      <c r="D143" t="inlineStr"/>
+      <c r="D143" s="10" t="inlineStr"/>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr">
+      <c r="A144" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:58:14</t>
         </is>
       </c>
-      <c r="B144" t="inlineStr">
+      <c r="B144" s="10" t="inlineStr">
         <is>
           <t>Wired Keyboard</t>
         </is>
       </c>
-      <c r="C144" t="inlineStr">
+      <c r="C144" s="10" t="inlineStr">
         <is>
           <t>add 2</t>
         </is>
       </c>
-      <c r="D144" t="inlineStr"/>
+      <c r="D144" s="10" t="inlineStr"/>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr">
+      <c r="A145" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:58:17</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr">
+      <c r="B145" s="10" t="inlineStr">
         <is>
           <t>Wireless KB &amp; Mouse</t>
         </is>
       </c>
-      <c r="C145" t="inlineStr">
+      <c r="C145" s="10" t="inlineStr">
         <is>
           <t>add 2</t>
         </is>
       </c>
-      <c r="D145" t="inlineStr"/>
+      <c r="D145" s="10" t="inlineStr"/>
     </row>
     <row r="146">
-      <c r="A146" t="inlineStr">
+      <c r="A146" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:58:17</t>
         </is>
       </c>
-      <c r="B146" t="inlineStr">
+      <c r="B146" s="10" t="inlineStr">
         <is>
           <t>Wireless KB &amp; Mouse</t>
         </is>
       </c>
-      <c r="C146" t="inlineStr">
+      <c r="C146" s="10" t="inlineStr">
         <is>
           <t>add 2</t>
         </is>
       </c>
-      <c r="D146" t="inlineStr"/>
+      <c r="D146" s="10" t="inlineStr"/>
     </row>
     <row r="147">
-      <c r="A147" t="inlineStr">
+      <c r="A147" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 00:59:50</t>
         </is>
       </c>
-      <c r="B147" t="inlineStr">
+      <c r="B147" s="10" t="inlineStr">
         <is>
           <t>Laptop x360 G8</t>
         </is>
       </c>
-      <c r="C147" t="inlineStr">
+      <c r="C147" s="10" t="inlineStr">
         <is>
           <t>add 1</t>
         </is>
       </c>
-      <c r="D147" t="inlineStr">
+      <c r="D147" s="10" t="inlineStr">
         <is>
           <t>SAN123456</t>
         </is>
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="inlineStr">
+      <c r="A148" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 01:00:02</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr">
+      <c r="B148" s="10" t="inlineStr">
         <is>
           <t>Laptop x360 G8</t>
         </is>
       </c>
-      <c r="C148" t="inlineStr">
+      <c r="C148" s="10" t="inlineStr">
         <is>
           <t>add 1</t>
         </is>
       </c>
-      <c r="D148" t="inlineStr">
+      <c r="D148" s="10" t="inlineStr">
         <is>
           <t>SAN123455</t>
         </is>
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="inlineStr">
+      <c r="A149" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 01:00:32</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr">
+      <c r="B149" s="10" t="inlineStr">
         <is>
           <t>Laptop x360 G8</t>
         </is>
       </c>
-      <c r="C149" t="inlineStr">
+      <c r="C149" s="10" t="inlineStr">
         <is>
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D149" t="inlineStr">
+      <c r="D149" s="10" t="inlineStr">
         <is>
           <t>SAN123455</t>
         </is>
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="inlineStr">
+      <c r="A150" s="10" t="inlineStr">
         <is>
           <t>2024-02-03 01:00:53</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr">
+      <c r="B150" s="10" t="inlineStr">
         <is>
           <t>Laptop x360 G8</t>
         </is>
       </c>
-      <c r="C150" t="inlineStr">
+      <c r="C150" s="10" t="inlineStr">
         <is>
           <t>subtract 1</t>
         </is>
       </c>
-      <c r="D150" t="inlineStr">
+      <c r="D150" s="10" t="inlineStr">
         <is>
           <t>SAN123456</t>
         </is>
       </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-03 21:12:38</t>
+        </is>
+      </c>
+      <c r="B151" s="10" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C151" s="10" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D151" s="10" t="inlineStr">
+        <is>
+          <t>SAN44</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="10" t="inlineStr">
+        <is>
+          <t>2024-02-03 21:13:21</t>
+        </is>
+      </c>
+      <c r="B152" s="10" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C152" s="10" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D152" s="10" t="inlineStr">
+        <is>
+          <t>SAN09090909</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:15:06</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>SAN343434</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:15:09</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>SAN454545</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:15:15</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G2</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:15:15</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G2</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>subtract 2</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:15:33</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>SAN454545</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:15:39</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>SAN343434</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:15:52</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>SAN222444</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:16:02</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Wired Keyboard</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:16:02</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Wired Keyboard</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:16:04</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Wired Mouse</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:16:04</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Wired Mouse</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2024-02-03 22:16:22</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wireless Headset Poly </t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr"/>
     </row>
     <row r="1048576" ht="12.75" customHeight="1" s="7"/>
   </sheetData>
@@ -5153,7 +5487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
@@ -5374,27 +5708,46 @@
       <c r="C16" s="10" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>g55f5g</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="10" t="inlineStr">
         <is>
           <t>INC4545454</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" s="10" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="10" t="inlineStr">
         <is>
           <t>445vv4</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="10" t="inlineStr">
         <is>
           <t>dfdffdfffd</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>g968g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>g968g6</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>TASK55555</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added All SANs log and Headsets log as options in the Data dropdown menu
</commit_message>
<xml_diff>
--- a/EUC_Perth_Assets.xlsx
+++ b/EUC_Perth_Assets.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="All SANs" sheetId="1" state="visible" r:id="rId1"/>
@@ -318,13 +318,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="25.42" customWidth="1" style="8" min="1" max="3"/>
   </cols>
@@ -347,14 +347,26 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1" s="9">
-      <c r="A2" s="11" t="n"/>
-      <c r="B2" s="11" t="n"/>
-      <c r="C2" s="11" t="n"/>
+      <c r="A2" s="11" t="inlineStr">
+        <is>
+          <t>SAN125045</t>
+        </is>
+      </c>
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C2" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:29:34</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="9">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>SAN125045</t>
+          <t>SAN125047</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -364,1353 +376,1320 @@
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>2024-01-10 16:29:34</t>
+          <t>2024-01-10 16:29:47</t>
         </is>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="9">
-      <c r="A4" s="8" t="inlineStr">
-        <is>
-          <t>SAN125047</t>
-        </is>
-      </c>
-      <c r="B4" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C4" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:29:47</t>
+      <c r="A4" s="11" t="inlineStr">
+        <is>
+          <t>SAN125043</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C4" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:29:53</t>
         </is>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="9">
-      <c r="A5" s="8" t="inlineStr">
-        <is>
-          <t>SAN125043</t>
-        </is>
-      </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C5" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:29:53</t>
+      <c r="A5" s="11" t="inlineStr">
+        <is>
+          <t>SAN125067</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C5" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:29:56</t>
         </is>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="9">
-      <c r="A6" s="8" t="inlineStr">
-        <is>
-          <t>SAN125067</t>
-        </is>
-      </c>
-      <c r="B6" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C6" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:29:56</t>
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>SAN125078</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:30:01</t>
         </is>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="9">
-      <c r="A7" s="8" t="inlineStr">
-        <is>
-          <t>SAN125078</t>
-        </is>
-      </c>
-      <c r="B7" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C7" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:30:01</t>
+      <c r="A7" s="11" t="inlineStr">
+        <is>
+          <t>SAN125060</t>
+        </is>
+      </c>
+      <c r="B7" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C7" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:30:05</t>
         </is>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="9">
-      <c r="A8" s="8" t="inlineStr">
-        <is>
-          <t>SAN125060</t>
-        </is>
-      </c>
-      <c r="B8" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:30:05</t>
+      <c r="A8" s="11" t="inlineStr">
+        <is>
+          <t>SAN125059</t>
+        </is>
+      </c>
+      <c r="B8" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C8" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:30:11</t>
         </is>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="9">
-      <c r="A9" s="8" t="inlineStr">
-        <is>
-          <t>SAN125059</t>
-        </is>
-      </c>
-      <c r="B9" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:30:11</t>
+      <c r="A9" s="11" t="inlineStr">
+        <is>
+          <t>SAN125065</t>
+        </is>
+      </c>
+      <c r="B9" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C9" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:30:17</t>
         </is>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="9">
-      <c r="A10" s="8" t="inlineStr">
-        <is>
-          <t>SAN125065</t>
-        </is>
-      </c>
-      <c r="B10" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C10" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:30:17</t>
+      <c r="A10" s="11" t="inlineStr">
+        <is>
+          <t>SAN125063</t>
+        </is>
+      </c>
+      <c r="B10" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:30:23</t>
         </is>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="9">
-      <c r="A11" s="8" t="inlineStr">
-        <is>
-          <t>SAN125063</t>
-        </is>
-      </c>
-      <c r="B11" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C11" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:30:23</t>
+      <c r="A11" s="11" t="inlineStr">
+        <is>
+          <t>SAN125064</t>
+        </is>
+      </c>
+      <c r="B11" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C11" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:30:29</t>
         </is>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="9">
-      <c r="A12" s="8" t="inlineStr">
-        <is>
-          <t>SAN125064</t>
-        </is>
-      </c>
-      <c r="B12" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C12" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:30:29</t>
+      <c r="A12" s="11" t="inlineStr">
+        <is>
+          <t>SAN125054</t>
+        </is>
+      </c>
+      <c r="B12" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C12" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:30:34</t>
         </is>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="9">
-      <c r="A13" s="8" t="inlineStr">
-        <is>
-          <t>SAN125054</t>
-        </is>
-      </c>
-      <c r="B13" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C13" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:30:34</t>
+      <c r="A13" s="11" t="inlineStr">
+        <is>
+          <t>SAN125061</t>
+        </is>
+      </c>
+      <c r="B13" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C13" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:30:45</t>
         </is>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="9">
-      <c r="A14" s="8" t="inlineStr">
-        <is>
-          <t>SAN125061</t>
-        </is>
-      </c>
-      <c r="B14" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C14" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:30:45</t>
+      <c r="A14" s="11" t="inlineStr">
+        <is>
+          <t>SAN125071</t>
+        </is>
+      </c>
+      <c r="B14" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C14" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:30:59</t>
         </is>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" s="9">
-      <c r="A15" s="8" t="inlineStr">
-        <is>
-          <t>SAN125071</t>
-        </is>
-      </c>
-      <c r="B15" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C15" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:30:59</t>
+      <c r="A15" s="11" t="inlineStr">
+        <is>
+          <t>SAN125072</t>
+        </is>
+      </c>
+      <c r="B15" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C15" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:31:09</t>
         </is>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" s="9">
-      <c r="A16" s="8" t="inlineStr">
-        <is>
-          <t>SAN125072</t>
-        </is>
-      </c>
-      <c r="B16" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C16" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:31:09</t>
+      <c r="A16" s="11" t="inlineStr">
+        <is>
+          <t>SAN125053</t>
+        </is>
+      </c>
+      <c r="B16" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C16" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:31:14</t>
         </is>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" s="9">
-      <c r="A17" s="8" t="inlineStr">
-        <is>
-          <t>SAN125053</t>
-        </is>
-      </c>
-      <c r="B17" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C17" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:31:14</t>
+      <c r="A17" s="11" t="inlineStr">
+        <is>
+          <t>SAN125077</t>
+        </is>
+      </c>
+      <c r="B17" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C17" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:31:23</t>
         </is>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1" s="9">
-      <c r="A18" s="8" t="inlineStr">
-        <is>
-          <t>SAN125077</t>
-        </is>
-      </c>
-      <c r="B18" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C18" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:31:23</t>
+      <c r="A18" s="11" t="inlineStr">
+        <is>
+          <t>SAN125076</t>
+        </is>
+      </c>
+      <c r="B18" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C18" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:31:28</t>
         </is>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1" s="9">
-      <c r="A19" s="8" t="inlineStr">
-        <is>
-          <t>SAN125076</t>
-        </is>
-      </c>
-      <c r="B19" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C19" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:31:28</t>
+      <c r="A19" s="11" t="inlineStr">
+        <is>
+          <t>SAN122589</t>
+        </is>
+      </c>
+      <c r="B19" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C19" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:39:28</t>
         </is>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1" s="9">
-      <c r="A20" s="8" t="inlineStr">
-        <is>
-          <t>SAN122589</t>
-        </is>
-      </c>
-      <c r="B20" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C20" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:39:28</t>
+      <c r="A20" s="11" t="inlineStr">
+        <is>
+          <t>SAN122596</t>
+        </is>
+      </c>
+      <c r="B20" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C20" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:39:32</t>
         </is>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1" s="9">
-      <c r="A21" s="8" t="inlineStr">
-        <is>
-          <t>SAN122596</t>
-        </is>
-      </c>
-      <c r="B21" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C21" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:39:32</t>
+      <c r="A21" s="11" t="inlineStr">
+        <is>
+          <t>SAN122603</t>
+        </is>
+      </c>
+      <c r="B21" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C21" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:39:40</t>
         </is>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1" s="9">
-      <c r="A22" s="8" t="inlineStr">
-        <is>
-          <t>SAN122603</t>
-        </is>
-      </c>
-      <c r="B22" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C22" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:39:40</t>
+      <c r="A22" s="11" t="inlineStr">
+        <is>
+          <t>SAN122611</t>
+        </is>
+      </c>
+      <c r="B22" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C22" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:39:47</t>
         </is>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1" s="9">
-      <c r="A23" s="8" t="inlineStr">
-        <is>
-          <t>SAN122611</t>
-        </is>
-      </c>
-      <c r="B23" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C23" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:39:47</t>
+      <c r="A23" s="11" t="inlineStr">
+        <is>
+          <t>SAN122590</t>
+        </is>
+      </c>
+      <c r="B23" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C23" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:39:53</t>
         </is>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1" s="9">
-      <c r="A24" s="8" t="inlineStr">
-        <is>
-          <t>SAN122590</t>
-        </is>
-      </c>
-      <c r="B24" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C24" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:39:53</t>
+      <c r="A24" s="11" t="inlineStr">
+        <is>
+          <t>SAN122593</t>
+        </is>
+      </c>
+      <c r="B24" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C24" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:40:16</t>
         </is>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1" s="9">
-      <c r="A25" s="8" t="inlineStr">
-        <is>
-          <t>SAN122593</t>
-        </is>
-      </c>
-      <c r="B25" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C25" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:40:16</t>
+      <c r="A25" s="11" t="inlineStr">
+        <is>
+          <t>SAN122597</t>
+        </is>
+      </c>
+      <c r="B25" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C25" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:40:40</t>
         </is>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1" s="9">
-      <c r="A26" s="8" t="inlineStr">
-        <is>
-          <t>SAN122597</t>
-        </is>
-      </c>
-      <c r="B26" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C26" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:40:40</t>
+      <c r="A26" s="11" t="inlineStr">
+        <is>
+          <t>SAN122602</t>
+        </is>
+      </c>
+      <c r="B26" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C26" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:40:49</t>
         </is>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1" s="9">
-      <c r="A27" s="8" t="inlineStr">
-        <is>
-          <t>SAN122602</t>
-        </is>
-      </c>
-      <c r="B27" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C27" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:40:49</t>
+      <c r="A27" s="11" t="inlineStr">
+        <is>
+          <t>SAN122610</t>
+        </is>
+      </c>
+      <c r="B27" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C27" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:40:53</t>
         </is>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1" s="9">
-      <c r="A28" s="8" t="inlineStr">
-        <is>
-          <t>SAN122610</t>
-        </is>
-      </c>
-      <c r="B28" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C28" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:40:53</t>
+      <c r="A28" s="11" t="inlineStr">
+        <is>
+          <t>SAN122599</t>
+        </is>
+      </c>
+      <c r="B28" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C28" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:40:58</t>
         </is>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1" s="9">
-      <c r="A29" s="8" t="inlineStr">
-        <is>
-          <t>SAN122599</t>
-        </is>
-      </c>
-      <c r="B29" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C29" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:40:58</t>
+      <c r="A29" s="11" t="inlineStr">
+        <is>
+          <t>SAN122592</t>
+        </is>
+      </c>
+      <c r="B29" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C29" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:41:03</t>
         </is>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1" s="9">
-      <c r="A30" s="8" t="inlineStr">
-        <is>
-          <t>SAN122592</t>
-        </is>
-      </c>
-      <c r="B30" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C30" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:41:03</t>
+      <c r="A30" s="11" t="inlineStr">
+        <is>
+          <t>SAN122607</t>
+        </is>
+      </c>
+      <c r="B30" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C30" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:41:08</t>
         </is>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1" s="9">
-      <c r="A31" s="8" t="inlineStr">
-        <is>
-          <t>SAN122607</t>
-        </is>
-      </c>
-      <c r="B31" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C31" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:41:08</t>
+      <c r="A31" s="11" t="inlineStr">
+        <is>
+          <t>SAN122608</t>
+        </is>
+      </c>
+      <c r="B31" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C31" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:41:15</t>
         </is>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1" s="9">
-      <c r="A32" s="8" t="inlineStr">
-        <is>
-          <t>SAN122608</t>
-        </is>
-      </c>
-      <c r="B32" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C32" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:41:15</t>
+      <c r="A32" s="11" t="inlineStr">
+        <is>
+          <t>SAN122598</t>
+        </is>
+      </c>
+      <c r="B32" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C32" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:41:20</t>
         </is>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1" s="9">
-      <c r="A33" s="8" t="inlineStr">
-        <is>
-          <t>SAN122598</t>
-        </is>
-      </c>
-      <c r="B33" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C33" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:41:20</t>
-        </is>
-      </c>
-    </row>
-    <row r="34" ht="12.75" customHeight="1" s="9">
-      <c r="A34" s="8" t="inlineStr">
+      <c r="A33" s="11" t="inlineStr">
         <is>
           <t>SAN122591</t>
         </is>
       </c>
-      <c r="B34" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C34" s="8" t="inlineStr">
+      <c r="B33" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C33" s="11" t="inlineStr">
         <is>
           <t>2024-01-10 16:41:26</t>
         </is>
       </c>
     </row>
+    <row r="34" ht="12" customHeight="1" s="9">
+      <c r="A34" s="11" t="inlineStr">
+        <is>
+          <t>SAN122613</t>
+        </is>
+      </c>
+      <c r="B34" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C34" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:41:42</t>
+        </is>
+      </c>
+    </row>
     <row r="35" ht="12" customHeight="1" s="9">
-      <c r="A35" s="8" t="inlineStr">
-        <is>
-          <t>SAN122613</t>
-        </is>
-      </c>
-      <c r="B35" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C35" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:41:42</t>
+      <c r="A35" s="11" t="inlineStr">
+        <is>
+          <t>SAN122604</t>
+        </is>
+      </c>
+      <c r="B35" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C35" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:41:50</t>
         </is>
       </c>
     </row>
     <row r="36" ht="12" customHeight="1" s="9">
-      <c r="A36" s="8" t="inlineStr">
-        <is>
-          <t>SAN122604</t>
-        </is>
-      </c>
-      <c r="B36" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C36" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:41:50</t>
+      <c r="A36" s="11" t="inlineStr">
+        <is>
+          <t>SAN122605</t>
+        </is>
+      </c>
+      <c r="B36" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C36" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:42:01</t>
         </is>
       </c>
     </row>
     <row r="37" ht="12" customHeight="1" s="9">
-      <c r="A37" s="8" t="inlineStr">
-        <is>
-          <t>SAN122605</t>
-        </is>
-      </c>
-      <c r="B37" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C37" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:42:01</t>
+      <c r="A37" s="11" t="inlineStr">
+        <is>
+          <t>SAN122606</t>
+        </is>
+      </c>
+      <c r="B37" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C37" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:42:07</t>
         </is>
       </c>
     </row>
     <row r="38" ht="12" customHeight="1" s="9">
-      <c r="A38" s="8" t="inlineStr">
-        <is>
-          <t>SAN122606</t>
-        </is>
-      </c>
-      <c r="B38" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C38" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:42:07</t>
+      <c r="A38" s="11" t="inlineStr">
+        <is>
+          <t>SAN122601</t>
+        </is>
+      </c>
+      <c r="B38" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C38" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:42:13</t>
         </is>
       </c>
     </row>
     <row r="39" ht="12" customHeight="1" s="9">
-      <c r="A39" s="8" t="inlineStr">
-        <is>
-          <t>SAN122601</t>
-        </is>
-      </c>
-      <c r="B39" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C39" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:42:13</t>
+      <c r="A39" s="11" t="inlineStr">
+        <is>
+          <t>SAN122595</t>
+        </is>
+      </c>
+      <c r="B39" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C39" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:42:19</t>
         </is>
       </c>
     </row>
     <row r="40" ht="12" customHeight="1" s="9">
-      <c r="A40" s="8" t="inlineStr">
-        <is>
-          <t>SAN122595</t>
-        </is>
-      </c>
-      <c r="B40" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C40" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:42:19</t>
+      <c r="A40" s="11" t="inlineStr">
+        <is>
+          <t>SAN122609</t>
+        </is>
+      </c>
+      <c r="B40" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C40" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:43:15</t>
         </is>
       </c>
     </row>
     <row r="41" ht="12" customHeight="1" s="9">
-      <c r="A41" s="8" t="inlineStr">
-        <is>
-          <t>SAN122609</t>
-        </is>
-      </c>
-      <c r="B41" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C41" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:43:15</t>
+      <c r="A41" s="11" t="inlineStr">
+        <is>
+          <t>SAN122594</t>
+        </is>
+      </c>
+      <c r="B41" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C41" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:43:21</t>
         </is>
       </c>
     </row>
     <row r="42" ht="12" customHeight="1" s="9">
-      <c r="A42" s="8" t="inlineStr">
-        <is>
-          <t>SAN122594</t>
-        </is>
-      </c>
-      <c r="B42" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C42" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:43:21</t>
+      <c r="A42" s="11" t="inlineStr">
+        <is>
+          <t>SAN122612</t>
+        </is>
+      </c>
+      <c r="B42" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C42" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:43:39</t>
         </is>
       </c>
     </row>
     <row r="43" ht="12" customHeight="1" s="9">
-      <c r="A43" s="8" t="inlineStr">
-        <is>
-          <t>SAN122612</t>
-        </is>
-      </c>
-      <c r="B43" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C43" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:43:39</t>
+      <c r="A43" s="11" t="inlineStr">
+        <is>
+          <t>SAN122304</t>
+        </is>
+      </c>
+      <c r="B43" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C43" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:43:46</t>
         </is>
       </c>
     </row>
     <row r="44" ht="12" customHeight="1" s="9">
-      <c r="A44" s="8" t="inlineStr">
-        <is>
-          <t>SAN122304</t>
-        </is>
-      </c>
-      <c r="B44" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C44" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:43:46</t>
+      <c r="A44" s="11" t="inlineStr">
+        <is>
+          <t>SAN122305</t>
+        </is>
+      </c>
+      <c r="B44" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C44" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:43:53</t>
         </is>
       </c>
     </row>
     <row r="45" ht="12" customHeight="1" s="9">
-      <c r="A45" s="8" t="inlineStr">
-        <is>
-          <t>SAN122305</t>
-        </is>
-      </c>
-      <c r="B45" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C45" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:43:53</t>
+      <c r="A45" s="11" t="inlineStr">
+        <is>
+          <t>SAN122600</t>
+        </is>
+      </c>
+      <c r="B45" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C45" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:44:23</t>
         </is>
       </c>
     </row>
     <row r="46" ht="12" customHeight="1" s="9">
-      <c r="A46" s="8" t="inlineStr">
-        <is>
-          <t>SAN122600</t>
-        </is>
-      </c>
-      <c r="B46" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C46" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:44:23</t>
+      <c r="A46" s="11" t="inlineStr">
+        <is>
+          <t>SAN121911</t>
+        </is>
+      </c>
+      <c r="B46" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C46" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:50:07</t>
         </is>
       </c>
     </row>
     <row r="47" ht="12" customHeight="1" s="9">
-      <c r="A47" s="8" t="inlineStr">
-        <is>
-          <t>SAN121911</t>
-        </is>
-      </c>
-      <c r="B47" s="8" t="inlineStr">
+      <c r="A47" s="11" t="inlineStr">
+        <is>
+          <t>SAN120358</t>
+        </is>
+      </c>
+      <c r="B47" s="11" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C47" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:50:07</t>
+      <c r="C47" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:50:19</t>
         </is>
       </c>
     </row>
     <row r="48" ht="12" customHeight="1" s="9">
-      <c r="A48" s="8" t="inlineStr">
-        <is>
-          <t>SAN120358</t>
-        </is>
-      </c>
-      <c r="B48" s="8" t="inlineStr">
+      <c r="A48" s="11" t="inlineStr">
+        <is>
+          <t>SAN121929</t>
+        </is>
+      </c>
+      <c r="B48" s="11" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C48" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:50:19</t>
+      <c r="C48" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:50:29</t>
         </is>
       </c>
     </row>
     <row r="49" ht="12" customHeight="1" s="9">
-      <c r="A49" s="8" t="inlineStr">
-        <is>
-          <t>SAN121929</t>
-        </is>
-      </c>
-      <c r="B49" s="8" t="inlineStr">
+      <c r="A49" s="11" t="inlineStr">
+        <is>
+          <t>SAN121895</t>
+        </is>
+      </c>
+      <c r="B49" s="11" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C49" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:50:29</t>
+      <c r="C49" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:50:38</t>
         </is>
       </c>
     </row>
     <row r="50" ht="12" customHeight="1" s="9">
-      <c r="A50" s="8" t="inlineStr">
-        <is>
-          <t>SAN121895</t>
-        </is>
-      </c>
-      <c r="B50" s="8" t="inlineStr">
+      <c r="A50" s="11" t="inlineStr">
+        <is>
+          <t>SAN120286</t>
+        </is>
+      </c>
+      <c r="B50" s="11" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C50" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:50:38</t>
+      <c r="C50" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:50:46</t>
         </is>
       </c>
     </row>
     <row r="51" ht="12" customHeight="1" s="9">
-      <c r="A51" s="8" t="inlineStr">
-        <is>
-          <t>SAN120286</t>
-        </is>
-      </c>
-      <c r="B51" s="8" t="inlineStr">
+      <c r="A51" s="11" t="inlineStr">
+        <is>
+          <t>SAN120342</t>
+        </is>
+      </c>
+      <c r="B51" s="11" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C51" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:50:46</t>
+      <c r="C51" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:50:57</t>
         </is>
       </c>
     </row>
     <row r="52" ht="12" customHeight="1" s="9">
-      <c r="A52" s="8" t="inlineStr">
-        <is>
-          <t>SAN120342</t>
-        </is>
-      </c>
-      <c r="B52" s="8" t="inlineStr">
+      <c r="A52" s="11" t="inlineStr">
+        <is>
+          <t>SAN106013</t>
+        </is>
+      </c>
+      <c r="B52" s="11" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C52" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:51:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" ht="12" customHeight="1" s="9">
+      <c r="A53" s="11" t="inlineStr">
+        <is>
+          <t>SAN106014</t>
+        </is>
+      </c>
+      <c r="B53" s="11" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C53" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:52:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="54" ht="12" customHeight="1" s="9">
+      <c r="A54" s="11" t="inlineStr">
+        <is>
+          <t>SAN106026</t>
+        </is>
+      </c>
+      <c r="B54" s="11" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C54" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:52:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" ht="12" customHeight="1" s="9">
+      <c r="A55" s="11" t="inlineStr">
+        <is>
+          <t>SAN106008</t>
+        </is>
+      </c>
+      <c r="B55" s="11" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C55" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-10 16:52:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" ht="12" customHeight="1" s="9">
+      <c r="A56" s="11" t="inlineStr">
+        <is>
+          <t>SAN111111</t>
+        </is>
+      </c>
+      <c r="B56" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C56" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-11 12:06:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="57" ht="12" customHeight="1" s="9">
+      <c r="A57" s="11" t="inlineStr">
+        <is>
+          <t>SAN120950</t>
+        </is>
+      </c>
+      <c r="B57" s="11" t="inlineStr">
         <is>
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="C52" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:50:57</t>
-        </is>
-      </c>
-    </row>
-    <row r="53" ht="12" customHeight="1" s="9">
-      <c r="A53" s="8" t="inlineStr">
-        <is>
-          <t>SAN106013</t>
-        </is>
-      </c>
-      <c r="B53" s="8" t="inlineStr">
+      <c r="C57" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-12 10:54:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" ht="12" customHeight="1" s="9">
+      <c r="A58" s="11" t="inlineStr">
+        <is>
+          <t>SAN120864</t>
+        </is>
+      </c>
+      <c r="B58" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C58" s="11" t="inlineStr">
+        <is>
+          <t>2024-01-12 10:54:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="59" ht="12" customHeight="1" s="9">
+      <c r="A59" s="11" t="inlineStr">
+        <is>
+          <t>SAN467985</t>
+        </is>
+      </c>
+      <c r="B59" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C59" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 19:51:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" ht="12" customHeight="1" s="9">
+      <c r="A60" s="11" t="inlineStr">
+        <is>
+          <t>SAN154856</t>
+        </is>
+      </c>
+      <c r="B60" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C60" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 19:51:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="61" ht="12" customHeight="1" s="9">
+      <c r="A61" s="11" t="inlineStr">
+        <is>
+          <t>SAN354687</t>
+        </is>
+      </c>
+      <c r="B61" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C61" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 19:51:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" ht="12" customHeight="1" s="9">
+      <c r="A62" s="11" t="inlineStr">
+        <is>
+          <t>SAN868686</t>
+        </is>
+      </c>
+      <c r="B62" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C62" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 20:27:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="63" ht="12" customHeight="1" s="9">
+      <c r="A63" s="11" t="inlineStr">
+        <is>
+          <t>SAN474747</t>
+        </is>
+      </c>
+      <c r="B63" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C63" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 20:27:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="64" ht="12" customHeight="1" s="9">
+      <c r="A64" s="11" t="inlineStr">
+        <is>
+          <t>SAN32323</t>
+        </is>
+      </c>
+      <c r="B64" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C64" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:00:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="65" ht="12" customHeight="1" s="9">
+      <c r="A65" s="11" t="inlineStr">
+        <is>
+          <t>SAN387876</t>
+        </is>
+      </c>
+      <c r="B65" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C65" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:17:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="66" ht="12" customHeight="1" s="9">
+      <c r="A66" s="11" t="inlineStr">
+        <is>
+          <t>SAN747474</t>
+        </is>
+      </c>
+      <c r="B66" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C66" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:17:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="67" ht="12" customHeight="1" s="9">
+      <c r="A67" s="11" t="inlineStr">
+        <is>
+          <t>SAN737373</t>
+        </is>
+      </c>
+      <c r="B67" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C67" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:18:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="68" ht="12" customHeight="1" s="9">
+      <c r="A68" s="11" t="inlineStr">
+        <is>
+          <t>SAN85685</t>
+        </is>
+      </c>
+      <c r="B68" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C68" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:19:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="69" ht="12" customHeight="1" s="9">
+      <c r="A69" s="11" t="inlineStr">
+        <is>
+          <t>SAN353535</t>
+        </is>
+      </c>
+      <c r="B69" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C69" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:20:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="70" ht="12" customHeight="1" s="9">
+      <c r="A70" s="11" t="inlineStr">
+        <is>
+          <t>SAN777777</t>
+        </is>
+      </c>
+      <c r="B70" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C70" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:20:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="71" ht="12" customHeight="1" s="9">
+      <c r="A71" s="11" t="inlineStr">
+        <is>
+          <t>SAN153759</t>
+        </is>
+      </c>
+      <c r="B71" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C71" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:22:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="72" ht="12" customHeight="1" s="9">
+      <c r="A72" s="11" t="inlineStr">
+        <is>
+          <t>SAN080808</t>
+        </is>
+      </c>
+      <c r="B72" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C72" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:23:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="73" ht="12" customHeight="1" s="9">
+      <c r="A73" s="11" t="inlineStr">
+        <is>
+          <t>SAN255443</t>
+        </is>
+      </c>
+      <c r="B73" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C73" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:23:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="74" ht="12" customHeight="1" s="9">
+      <c r="A74" s="11" t="inlineStr">
+        <is>
+          <t>SAN323232</t>
+        </is>
+      </c>
+      <c r="B74" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C74" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:24:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="75" ht="12" customHeight="1" s="9">
+      <c r="A75" s="11" t="inlineStr">
+        <is>
+          <t>SAN111888</t>
+        </is>
+      </c>
+      <c r="B75" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C75" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:26:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="76" ht="12" customHeight="1" s="9">
+      <c r="A76" s="11" t="inlineStr">
+        <is>
+          <t>SAN797979</t>
+        </is>
+      </c>
+      <c r="B76" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C76" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 21:53:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="77" ht="12" customHeight="1" s="9">
+      <c r="A77" s="11" t="inlineStr">
+        <is>
+          <t>SAN323233</t>
+        </is>
+      </c>
+      <c r="B77" s="11" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C77" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 22:25:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="78" ht="12" customHeight="1" s="9">
+      <c r="A78" s="11" t="inlineStr">
+        <is>
+          <t>SAN632546</t>
+        </is>
+      </c>
+      <c r="B78" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C78" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 22:25:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="79" ht="12" customHeight="1" s="9">
+      <c r="A79" s="11" t="inlineStr">
+        <is>
+          <t>SAN642456</t>
+        </is>
+      </c>
+      <c r="B79" s="11" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C79" s="11" t="inlineStr">
+        <is>
+          <t>2024-02-04 22:25:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="80" ht="12" customHeight="1" s="9">
+      <c r="A80" s="11" t="inlineStr">
+        <is>
+          <t>SAN000666</t>
+        </is>
+      </c>
+      <c r="B80" s="11" t="inlineStr">
         <is>
           <t>Laptop x360 G8</t>
         </is>
       </c>
-      <c r="C53" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:51:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="54" ht="12" customHeight="1" s="9">
-      <c r="A54" s="8" t="inlineStr">
-        <is>
-          <t>SAN106014</t>
-        </is>
-      </c>
-      <c r="B54" s="8" t="inlineStr">
-        <is>
-          <t>Laptop x360 G8</t>
-        </is>
-      </c>
-      <c r="C54" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:52:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="55" ht="12" customHeight="1" s="9">
-      <c r="A55" s="8" t="inlineStr">
-        <is>
-          <t>SAN106026</t>
-        </is>
-      </c>
-      <c r="B55" s="8" t="inlineStr">
-        <is>
-          <t>Laptop x360 G8</t>
-        </is>
-      </c>
-      <c r="C55" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:52:08</t>
-        </is>
-      </c>
-    </row>
-    <row r="56" ht="12" customHeight="1" s="9">
-      <c r="A56" s="8" t="inlineStr">
-        <is>
-          <t>SAN106008</t>
-        </is>
-      </c>
-      <c r="B56" s="8" t="inlineStr">
-        <is>
-          <t>Laptop x360 G8</t>
-        </is>
-      </c>
-      <c r="C56" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-10 16:52:17</t>
-        </is>
-      </c>
-    </row>
-    <row r="57" ht="12" customHeight="1" s="9">
-      <c r="A57" s="8" t="inlineStr">
-        <is>
-          <t>SAN111111</t>
-        </is>
-      </c>
-      <c r="B57" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C57" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-11 12:06:10</t>
-        </is>
-      </c>
-    </row>
-    <row r="58" ht="12" customHeight="1" s="9">
-      <c r="A58" s="8" t="inlineStr">
-        <is>
-          <t>SAN120950</t>
-        </is>
-      </c>
-      <c r="B58" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G9</t>
-        </is>
-      </c>
-      <c r="C58" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-12 10:54:13</t>
-        </is>
-      </c>
-    </row>
-    <row r="59" ht="12" customHeight="1" s="9">
-      <c r="A59" s="8" t="inlineStr">
-        <is>
-          <t>SAN120864</t>
-        </is>
-      </c>
-      <c r="B59" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G9</t>
-        </is>
-      </c>
-      <c r="C59" s="8" t="inlineStr">
-        <is>
-          <t>2024-01-12 10:54:20</t>
-        </is>
-      </c>
-    </row>
-    <row r="60" ht="12" customHeight="1" s="9">
-      <c r="A60" s="12" t="inlineStr">
-        <is>
-          <t>SAN467985</t>
-        </is>
-      </c>
-      <c r="B60" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C60" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 19:51:04</t>
-        </is>
-      </c>
-    </row>
-    <row r="61" ht="12" customHeight="1" s="9">
-      <c r="A61" s="12" t="inlineStr">
-        <is>
-          <t>SAN154856</t>
-        </is>
-      </c>
-      <c r="B61" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C61" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 19:51:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="62" ht="12" customHeight="1" s="9">
-      <c r="A62" s="12" t="inlineStr">
-        <is>
-          <t>SAN354687</t>
-        </is>
-      </c>
-      <c r="B62" s="12" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C62" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 19:51:17</t>
-        </is>
-      </c>
-    </row>
-    <row r="63" ht="12" customHeight="1" s="9">
-      <c r="A63" s="12" t="inlineStr">
-        <is>
-          <t>SAN868686</t>
-        </is>
-      </c>
-      <c r="B63" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C63" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 20:27:07</t>
-        </is>
-      </c>
-    </row>
-    <row r="64" ht="12" customHeight="1" s="9">
-      <c r="A64" s="12" t="inlineStr">
-        <is>
-          <t>SAN474747</t>
-        </is>
-      </c>
-      <c r="B64" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C64" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 20:27:21</t>
-        </is>
-      </c>
-    </row>
-    <row r="65" ht="12" customHeight="1" s="9">
-      <c r="A65" s="12" t="inlineStr">
-        <is>
-          <t>SAN32323</t>
-        </is>
-      </c>
-      <c r="B65" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C65" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:00:10</t>
-        </is>
-      </c>
-    </row>
-    <row r="66" ht="12" customHeight="1" s="9">
-      <c r="A66" s="12" t="inlineStr">
-        <is>
-          <t>SAN387876</t>
-        </is>
-      </c>
-      <c r="B66" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C66" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:17:22</t>
-        </is>
-      </c>
-    </row>
-    <row r="67" ht="12" customHeight="1" s="9">
-      <c r="A67" s="12" t="inlineStr">
-        <is>
-          <t>SAN747474</t>
-        </is>
-      </c>
-      <c r="B67" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C67" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:17:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="68" ht="12" customHeight="1" s="9">
-      <c r="A68" s="12" t="inlineStr">
-        <is>
-          <t>SAN737373</t>
-        </is>
-      </c>
-      <c r="B68" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C68" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:18:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="69" ht="12" customHeight="1" s="9">
-      <c r="A69" s="12" t="inlineStr">
-        <is>
-          <t>SAN85685</t>
-        </is>
-      </c>
-      <c r="B69" s="12" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C69" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:19:02</t>
-        </is>
-      </c>
-    </row>
-    <row r="70" ht="12" customHeight="1" s="9">
-      <c r="A70" s="12" t="inlineStr">
-        <is>
-          <t>SAN353535</t>
-        </is>
-      </c>
-      <c r="B70" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C70" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:20:50</t>
-        </is>
-      </c>
-    </row>
-    <row r="71" ht="12" customHeight="1" s="9">
-      <c r="A71" s="12" t="inlineStr">
-        <is>
-          <t>SAN777777</t>
-        </is>
-      </c>
-      <c r="B71" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C71" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:20:57</t>
-        </is>
-      </c>
-    </row>
-    <row r="72" ht="12" customHeight="1" s="9">
-      <c r="A72" s="12" t="inlineStr">
-        <is>
-          <t>SAN153759</t>
-        </is>
-      </c>
-      <c r="B72" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C72" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:22:59</t>
-        </is>
-      </c>
-    </row>
-    <row r="73" ht="12" customHeight="1" s="9">
-      <c r="A73" s="12" t="inlineStr">
-        <is>
-          <t>SAN080808</t>
-        </is>
-      </c>
-      <c r="B73" s="12" t="inlineStr">
-        <is>
-          <t>Laptop 840 G9</t>
-        </is>
-      </c>
-      <c r="C73" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:23:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="74" ht="12" customHeight="1" s="9">
-      <c r="A74" s="12" t="inlineStr">
-        <is>
-          <t>SAN255443</t>
-        </is>
-      </c>
-      <c r="B74" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C74" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:23:51</t>
-        </is>
-      </c>
-    </row>
-    <row r="75" ht="12" customHeight="1" s="9">
-      <c r="A75" s="12" t="inlineStr">
-        <is>
-          <t>SAN323232</t>
-        </is>
-      </c>
-      <c r="B75" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C75" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:24:49</t>
-        </is>
-      </c>
-    </row>
-    <row r="76" ht="12" customHeight="1" s="9">
-      <c r="A76" s="12" t="inlineStr">
-        <is>
-          <t>SAN111888</t>
-        </is>
-      </c>
-      <c r="B76" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C76" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:26:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="77" ht="12" customHeight="1" s="9">
-      <c r="A77" s="12" t="inlineStr">
-        <is>
-          <t>SAN797979</t>
-        </is>
-      </c>
-      <c r="B77" s="12" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C77" s="12" t="inlineStr">
-        <is>
-          <t>2024-02-04 21:53:39</t>
-        </is>
-      </c>
-    </row>
-    <row r="78" ht="12" customHeight="1" s="9">
-      <c r="A78" s="8" t="inlineStr">
-        <is>
-          <t>SAN323233</t>
-        </is>
-      </c>
-      <c r="B78" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C78" s="8" t="inlineStr">
-        <is>
-          <t>2024-02-04 22:25:08</t>
-        </is>
-      </c>
-    </row>
-    <row r="79" ht="12" customHeight="1" s="9">
-      <c r="A79" s="8" t="inlineStr">
-        <is>
-          <t>SAN632546</t>
-        </is>
-      </c>
-      <c r="B79" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G10</t>
-        </is>
-      </c>
-      <c r="C79" s="8" t="inlineStr">
-        <is>
-          <t>2024-02-04 22:25:21</t>
-        </is>
-      </c>
-    </row>
-    <row r="80" ht="12" customHeight="1" s="9">
-      <c r="A80" s="8" t="inlineStr">
-        <is>
-          <t>SAN642456</t>
-        </is>
-      </c>
-      <c r="B80" s="8" t="inlineStr">
-        <is>
-          <t>Laptop 840 G9</t>
-        </is>
-      </c>
-      <c r="C80" s="8" t="inlineStr">
-        <is>
-          <t>2024-02-04 22:25:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="81" ht="12" customHeight="1" s="9">
-      <c r="A81" s="8" t="inlineStr">
-        <is>
-          <t>SAN000666</t>
-        </is>
-      </c>
-      <c r="B81" s="8" t="inlineStr">
-        <is>
-          <t>Laptop x360 G8</t>
-        </is>
-      </c>
-      <c r="C81" s="8" t="inlineStr">
+      <c r="C80" s="11" t="inlineStr">
         <is>
           <t>2024-02-04 22:25:41</t>
         </is>
       </c>
     </row>
-    <row r="82" ht="12" customHeight="1" s="9">
-      <c r="A82" s="8" t="inlineStr">
-        <is>
-          <t>SAN232323</t>
-        </is>
-      </c>
-      <c r="B82" s="8" t="inlineStr">
-        <is>
-          <t>Desktop Mini G9</t>
-        </is>
-      </c>
-      <c r="C82" s="8" t="inlineStr">
-        <is>
-          <t>2024-02-04 22:46:28</t>
-        </is>
-      </c>
-    </row>
+    <row r="81" ht="12" customHeight="1" s="9"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1767,10 +1746,10 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>24</v>
-      </c>
-      <c r="C2" s="8" t="n">
-        <v>25</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="9">
@@ -1910,10 +1889,10 @@
         </is>
       </c>
       <c r="B13" s="8" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C13" s="8" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="9">
@@ -1989,7 +1968,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D167"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A131" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
@@ -5255,23 +5234,61 @@
         </is>
       </c>
     </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
+    <row r="165" ht="12" customHeight="1" s="9">
+      <c r="A165" s="12" t="inlineStr">
         <is>
           <t>2024-02-04 23:01:45</t>
         </is>
       </c>
-      <c r="B165" t="inlineStr">
+      <c r="B165" s="12" t="inlineStr">
         <is>
           <t>Wired Headset Poly</t>
         </is>
       </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>add 1</t>
-        </is>
-      </c>
-      <c r="D165" t="inlineStr"/>
+      <c r="C165" s="12" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="166" ht="12" customHeight="1" s="9">
+      <c r="A166" s="12" t="inlineStr">
+        <is>
+          <t>2024-02-04 23:11:06</t>
+        </is>
+      </c>
+      <c r="B166" s="12" t="inlineStr">
+        <is>
+          <t>Wired Headset Poly</t>
+        </is>
+      </c>
+      <c r="C166" s="12" t="inlineStr">
+        <is>
+          <t>add 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2024-02-04 23:16:42</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Desktop Mini G9</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>subtract 1</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>SAN232323</t>
+        </is>
+      </c>
     </row>
     <row r="1048576" ht="12.75" customHeight="1" s="9"/>
   </sheetData>
@@ -5753,10 +5770,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.453125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5782,18 +5799,29 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1" s="9">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="12" t="inlineStr">
         <is>
           <t>4343vd</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="12" t="inlineStr">
         <is>
           <t>RITM343434</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1" s="9"/>
+    <row r="3" ht="12.75" customHeight="1" s="9">
+      <c r="A3" s="12" t="inlineStr">
+        <is>
+          <t>we34df</t>
+        </is>
+      </c>
+      <c r="B3" s="12" t="inlineStr">
+        <is>
+          <t>RITM3333333</t>
+        </is>
+      </c>
+    </row>
     <row r="4" ht="12.75" customHeight="1" s="9"/>
     <row r="5" ht="12.75" customHeight="1" s="9"/>
     <row r="6" ht="12.75" customHeight="1" s="9"/>

</xml_diff>